<commit_message>
POCOR-7382: code enhance for class template student performance summary | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/class_profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/class_profile_template.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umairah/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FE529C4-6676-854E-BE32-025034804EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32680" windowHeight="15920" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="29040" windowHeight="15915" tabRatio="862" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Student Performance Summary" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,82 +20,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{F01695D2-B671-4E84-9F87-A62CD3489B50}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>First Name + Middle Name + Third Name + Last Name</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{1D9C0F74-2025-4507-A482-610EFCC338CD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Please account for case when subjects can have different weights. Simple average may not always work</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
   <si>
@@ -432,8 +351,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -494,19 +413,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -662,10 +568,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -680,10 +586,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -814,7 +720,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -846,27 +752,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -898,24 +786,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1091,31 +961,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="63.1640625" customWidth="1"/>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="1" max="1" width="63.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="61.33203125" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="61.28515625" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
     <col min="7" max="7" width="58" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="18" width="39.5" customWidth="1"/>
-    <col min="19" max="27" width="41.83203125" customWidth="1"/>
-    <col min="28" max="256" width="39.6640625" customWidth="1"/>
-    <col min="257" max="1023" width="16.1640625" customWidth="1"/>
-    <col min="1024" max="1025" width="11.6640625" customWidth="1"/>
+    <col min="9" max="18" width="39.42578125" customWidth="1"/>
+    <col min="19" max="27" width="41.85546875" customWidth="1"/>
+    <col min="28" max="256" width="39.7109375" customWidth="1"/>
+    <col min="257" max="1023" width="16.140625" customWidth="1"/>
+    <col min="1024" max="1025" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:256" ht="15" customHeight="1">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1006,7 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
     </row>
-    <row r="2" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="25.5" customHeight="1">
       <c r="A2" s="29"/>
       <c r="B2" s="30" t="s">
         <v>1</v>
@@ -1396,7 +1266,7 @@
       <c r="IU2" s="2"/>
       <c r="IV2" s="2"/>
     </row>
-    <row r="3" spans="1:256" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="25.5" customHeight="1">
       <c r="A3" s="29"/>
       <c r="B3" s="31" t="s">
         <v>2</v>
@@ -1656,7 +1526,7 @@
       <c r="IU3" s="2"/>
       <c r="IV3" s="2"/>
     </row>
-    <row r="4" spans="1:256" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:256" ht="22.5" customHeight="1">
       <c r="A4" s="29"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1675,7 +1545,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:256" ht="15.75" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1695,7 +1565,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="12" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -1719,7 +1589,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="12" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
@@ -1743,7 +1613,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:256" ht="12" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1767,7 +1637,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:256" ht="12" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
@@ -1791,7 +1661,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:256" ht="12" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1815,7 +1685,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:256" ht="12" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
@@ -2077,7 +1947,7 @@
       <c r="IU11" s="2"/>
       <c r="IV11" s="2"/>
     </row>
-    <row r="12" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:256" ht="16.5" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2335,7 +2205,7 @@
       <c r="IU12" s="2"/>
       <c r="IV12" s="2"/>
     </row>
-    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:256" ht="16.5" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
@@ -2597,7 +2467,7 @@
       <c r="IU13" s="2"/>
       <c r="IV13" s="2"/>
     </row>
-    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="16.5" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
@@ -2859,7 +2729,7 @@
       <c r="IU14" s="2"/>
       <c r="IV14" s="2"/>
     </row>
-    <row r="15" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:256" ht="12" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
@@ -3121,7 +2991,7 @@
       <c r="IU15" s="2"/>
       <c r="IV15" s="2"/>
     </row>
-    <row r="16" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:256" ht="12" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
@@ -3383,7 +3253,7 @@
       <c r="IU16" s="2"/>
       <c r="IV16" s="2"/>
     </row>
-    <row r="17" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:256" ht="12" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
@@ -3645,7 +3515,7 @@
       <c r="IU17" s="2"/>
       <c r="IV17" s="2"/>
     </row>
-    <row r="18" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:256" ht="12" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>25</v>
       </c>
@@ -3907,7 +3777,7 @@
       <c r="IU18" s="2"/>
       <c r="IV18" s="2"/>
     </row>
-    <row r="19" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:256" ht="12" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>27</v>
       </c>
@@ -4169,7 +4039,7 @@
       <c r="IU19" s="2"/>
       <c r="IV19" s="2"/>
     </row>
-    <row r="20" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:256" ht="12" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>15</v>
       </c>
@@ -4431,7 +4301,7 @@
       <c r="IU20" s="2"/>
       <c r="IV20" s="2"/>
     </row>
-    <row r="21" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:256" ht="12" customHeight="1">
       <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
@@ -4693,7 +4563,7 @@
       <c r="IU21" s="2"/>
       <c r="IV21" s="2"/>
     </row>
-    <row r="22" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:256" ht="12" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
@@ -4955,7 +4825,7 @@
       <c r="IU22" s="2"/>
       <c r="IV22" s="2"/>
     </row>
-    <row r="23" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:256" ht="12" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>33</v>
       </c>
@@ -5217,7 +5087,7 @@
       <c r="IU23" s="2"/>
       <c r="IV23" s="2"/>
     </row>
-    <row r="24" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:256" ht="12" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
@@ -5479,7 +5349,7 @@
       <c r="IU24" s="2"/>
       <c r="IV24" s="2"/>
     </row>
-    <row r="25" spans="1:256" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:256" ht="12" customHeight="1">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="19"/>
@@ -5737,25 +5607,25 @@
       <c r="IU25" s="2"/>
       <c r="IV25" s="2"/>
     </row>
-    <row r="26" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="27" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="28" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="29" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="30" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="31" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="32" spans="1:256" ht="15.95" customHeight="1"/>
+    <row r="33" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="34" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="35" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="36" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="37" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="38" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="39" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="40" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="41" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="42" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="43" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="44" spans="1:16" ht="15.95" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
@@ -5775,7 +5645,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" ht="15.95" customHeight="1">
       <c r="A45" s="17" t="s">
         <v>39</v>
       </c>
@@ -5825,7 +5695,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" ht="15.95" customHeight="1">
       <c r="A46" s="18" t="s">
         <v>55</v>
       </c>
@@ -5875,77 +5745,77 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="48" spans="1:16" ht="15.95" customHeight="1"/>
+    <row r="49" ht="15.95" customHeight="1"/>
+    <row r="50" ht="15.95" customHeight="1"/>
+    <row r="51" ht="15.95" customHeight="1"/>
+    <row r="52" ht="15.95" customHeight="1"/>
+    <row r="53" ht="15.95" customHeight="1"/>
+    <row r="54" ht="15.95" customHeight="1"/>
+    <row r="55" ht="15.95" customHeight="1"/>
+    <row r="56" ht="15.95" customHeight="1"/>
+    <row r="57" ht="15.95" customHeight="1"/>
+    <row r="58" ht="15.95" customHeight="1"/>
+    <row r="59" ht="15.95" customHeight="1"/>
+    <row r="60" ht="15.95" customHeight="1"/>
+    <row r="61" ht="15.95" customHeight="1"/>
+    <row r="62" ht="15.95" customHeight="1"/>
+    <row r="63" ht="15.95" customHeight="1"/>
+    <row r="64" ht="15.95" customHeight="1"/>
+    <row r="65" ht="15.95" customHeight="1"/>
+    <row r="66" ht="15.95" customHeight="1"/>
+    <row r="67" ht="15.95" customHeight="1"/>
+    <row r="68" ht="15.95" customHeight="1"/>
+    <row r="69" ht="15.95" customHeight="1"/>
+    <row r="70" ht="15.95" customHeight="1"/>
+    <row r="71" ht="15.95" customHeight="1"/>
+    <row r="72" ht="15.95" customHeight="1"/>
+    <row r="73" ht="15.95" customHeight="1"/>
+    <row r="74" ht="15.95" customHeight="1"/>
+    <row r="75" ht="15.95" customHeight="1"/>
+    <row r="76" ht="15.95" customHeight="1"/>
+    <row r="77" ht="15.95" customHeight="1"/>
+    <row r="78" ht="15.95" customHeight="1"/>
+    <row r="79" ht="15.95" customHeight="1"/>
+    <row r="80" ht="15.95" customHeight="1"/>
+    <row r="81" ht="15.95" customHeight="1"/>
+    <row r="82" ht="15.95" customHeight="1"/>
+    <row r="83" ht="15.95" customHeight="1"/>
+    <row r="84" ht="15.95" customHeight="1"/>
+    <row r="85" ht="15.95" customHeight="1"/>
+    <row r="86" ht="15.95" customHeight="1"/>
+    <row r="87" ht="15.95" customHeight="1"/>
+    <row r="88" ht="15.95" customHeight="1"/>
+    <row r="89" ht="15.95" customHeight="1"/>
+    <row r="90" ht="15.95" customHeight="1"/>
+    <row r="91" ht="15.95" customHeight="1"/>
+    <row r="92" ht="15.95" customHeight="1"/>
+    <row r="93" ht="15.95" customHeight="1"/>
+    <row r="94" ht="15.95" customHeight="1"/>
+    <row r="95" ht="15.95" customHeight="1"/>
+    <row r="96" ht="15.95" customHeight="1"/>
+    <row r="97" ht="15.95" customHeight="1"/>
+    <row r="98" ht="15.95" customHeight="1"/>
+    <row r="99" ht="15.95" customHeight="1"/>
+    <row r="100" ht="15.95" customHeight="1"/>
+    <row r="101" ht="15.95" customHeight="1"/>
+    <row r="102" ht="15.95" customHeight="1"/>
+    <row r="103" ht="15.95" customHeight="1"/>
+    <row r="104" ht="15.95" customHeight="1"/>
+    <row r="105" ht="15.95" customHeight="1"/>
+    <row r="106" ht="15.95" customHeight="1"/>
+    <row r="107" ht="15.95" customHeight="1"/>
+    <row r="108" ht="15.95" customHeight="1"/>
+    <row r="109" ht="15.95" customHeight="1"/>
+    <row r="110" ht="15.95" customHeight="1"/>
+    <row r="111" ht="15.95" customHeight="1"/>
+    <row r="112" ht="15.95" customHeight="1"/>
+    <row r="113" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="114" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="115" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="116" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="117" spans="1:6" ht="15.95" customHeight="1">
       <c r="A117" s="1" t="s">
         <v>37</v>
       </c>
@@ -5955,7 +5825,7 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:6" ht="15.95" customHeight="1">
       <c r="A118" s="17" t="s">
         <v>71</v>
       </c>
@@ -5975,7 +5845,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:6" ht="15.95" customHeight="1">
       <c r="A119" s="18" t="s">
         <v>77</v>
       </c>
@@ -5995,874 +5865,874 @@
         <v>82</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="121" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="122" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="123" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="124" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="125" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="126" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="127" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="128" spans="1:6" ht="15.95" customHeight="1"/>
+    <row r="129" ht="15.95" customHeight="1"/>
+    <row r="130" ht="15.95" customHeight="1"/>
+    <row r="131" ht="15.95" customHeight="1"/>
+    <row r="132" ht="15.95" customHeight="1"/>
+    <row r="133" ht="15.95" customHeight="1"/>
+    <row r="134" ht="15.95" customHeight="1"/>
+    <row r="135" ht="15.95" customHeight="1"/>
+    <row r="136" ht="15.95" customHeight="1"/>
+    <row r="137" ht="15.95" customHeight="1"/>
+    <row r="138" ht="15.95" customHeight="1"/>
+    <row r="139" ht="15.95" customHeight="1"/>
+    <row r="140" ht="15.95" customHeight="1"/>
+    <row r="141" ht="15.95" customHeight="1"/>
+    <row r="142" ht="15.95" customHeight="1"/>
+    <row r="143" ht="15.95" customHeight="1"/>
+    <row r="144" ht="15.95" customHeight="1"/>
+    <row r="145" ht="15.95" customHeight="1"/>
+    <row r="146" ht="15.95" customHeight="1"/>
+    <row r="147" ht="15.95" customHeight="1"/>
+    <row r="148" ht="15.95" customHeight="1"/>
+    <row r="149" ht="15.95" customHeight="1"/>
+    <row r="150" ht="15.95" customHeight="1"/>
+    <row r="151" ht="15.95" customHeight="1"/>
+    <row r="152" ht="15.95" customHeight="1"/>
+    <row r="153" ht="15.95" customHeight="1"/>
+    <row r="154" ht="15.95" customHeight="1"/>
+    <row r="155" ht="15.95" customHeight="1"/>
+    <row r="156" ht="15.95" customHeight="1"/>
+    <row r="157" ht="15.95" customHeight="1"/>
+    <row r="158" ht="15.95" customHeight="1"/>
+    <row r="159" ht="15.95" customHeight="1"/>
+    <row r="160" ht="15.95" customHeight="1"/>
+    <row r="161" ht="15.95" customHeight="1"/>
+    <row r="162" ht="15.95" customHeight="1"/>
+    <row r="163" ht="15.95" customHeight="1"/>
+    <row r="164" ht="15.95" customHeight="1"/>
+    <row r="165" ht="15.95" customHeight="1"/>
+    <row r="166" ht="15.95" customHeight="1"/>
+    <row r="167" ht="15.95" customHeight="1"/>
+    <row r="168" ht="15.95" customHeight="1"/>
+    <row r="169" ht="15.95" customHeight="1"/>
+    <row r="170" ht="15.95" customHeight="1"/>
+    <row r="171" ht="15.95" customHeight="1"/>
+    <row r="172" ht="15.95" customHeight="1"/>
+    <row r="173" ht="15.95" customHeight="1"/>
+    <row r="174" ht="15.95" customHeight="1"/>
+    <row r="175" ht="15.95" customHeight="1"/>
+    <row r="176" ht="15.95" customHeight="1"/>
+    <row r="177" ht="15.95" customHeight="1"/>
+    <row r="178" ht="15.95" customHeight="1"/>
+    <row r="179" ht="15.95" customHeight="1"/>
+    <row r="180" ht="15.95" customHeight="1"/>
+    <row r="181" ht="15.95" customHeight="1"/>
+    <row r="182" ht="15.95" customHeight="1"/>
+    <row r="183" ht="15.95" customHeight="1"/>
+    <row r="184" ht="15.95" customHeight="1"/>
+    <row r="185" ht="15.95" customHeight="1"/>
+    <row r="186" ht="15.95" customHeight="1"/>
+    <row r="187" ht="15.95" customHeight="1"/>
+    <row r="188" ht="15.95" customHeight="1"/>
+    <row r="189" ht="15.95" customHeight="1"/>
+    <row r="190" ht="15.95" customHeight="1"/>
+    <row r="191" ht="15.95" customHeight="1"/>
+    <row r="192" ht="15.95" customHeight="1"/>
+    <row r="193" ht="15.95" customHeight="1"/>
+    <row r="194" ht="15.95" customHeight="1"/>
+    <row r="195" ht="15.95" customHeight="1"/>
+    <row r="196" ht="15.95" customHeight="1"/>
+    <row r="197" ht="15.95" customHeight="1"/>
+    <row r="198" ht="15.95" customHeight="1"/>
+    <row r="199" ht="15.95" customHeight="1"/>
+    <row r="200" ht="15.95" customHeight="1"/>
+    <row r="201" ht="15.95" customHeight="1"/>
+    <row r="202" ht="15.95" customHeight="1"/>
+    <row r="203" ht="15.95" customHeight="1"/>
+    <row r="204" ht="15.95" customHeight="1"/>
+    <row r="205" ht="15.95" customHeight="1"/>
+    <row r="206" ht="15.95" customHeight="1"/>
+    <row r="207" ht="15.95" customHeight="1"/>
+    <row r="208" ht="15.95" customHeight="1"/>
+    <row r="209" ht="15.95" customHeight="1"/>
+    <row r="210" ht="15.95" customHeight="1"/>
+    <row r="211" ht="15.95" customHeight="1"/>
+    <row r="212" ht="15.95" customHeight="1"/>
+    <row r="213" ht="15.95" customHeight="1"/>
+    <row r="214" ht="15.95" customHeight="1"/>
+    <row r="215" ht="15.95" customHeight="1"/>
+    <row r="216" ht="15.95" customHeight="1"/>
+    <row r="217" ht="15.95" customHeight="1"/>
+    <row r="218" ht="15.95" customHeight="1"/>
+    <row r="219" ht="15.95" customHeight="1"/>
+    <row r="220" ht="15.95" customHeight="1"/>
+    <row r="221" ht="15.95" customHeight="1"/>
+    <row r="222" ht="15.95" customHeight="1"/>
+    <row r="223" ht="15.95" customHeight="1"/>
+    <row r="224" ht="15.95" customHeight="1"/>
+    <row r="225" ht="15.95" customHeight="1"/>
+    <row r="226" ht="15.95" customHeight="1"/>
+    <row r="227" ht="15.95" customHeight="1"/>
+    <row r="228" ht="15.95" customHeight="1"/>
+    <row r="229" ht="15.95" customHeight="1"/>
+    <row r="230" ht="15.95" customHeight="1"/>
+    <row r="231" ht="15.95" customHeight="1"/>
+    <row r="232" ht="15.95" customHeight="1"/>
+    <row r="233" ht="15.95" customHeight="1"/>
+    <row r="234" ht="15.95" customHeight="1"/>
+    <row r="235" ht="15.95" customHeight="1"/>
+    <row r="236" ht="15.95" customHeight="1"/>
+    <row r="237" ht="15.95" customHeight="1"/>
+    <row r="238" ht="15.95" customHeight="1"/>
+    <row r="239" ht="15.95" customHeight="1"/>
+    <row r="240" ht="15.95" customHeight="1"/>
+    <row r="241" ht="15.95" customHeight="1"/>
+    <row r="242" ht="15.95" customHeight="1"/>
+    <row r="243" ht="15.95" customHeight="1"/>
+    <row r="244" ht="15.95" customHeight="1"/>
+    <row r="245" ht="15.95" customHeight="1"/>
+    <row r="246" ht="15.95" customHeight="1"/>
+    <row r="247" ht="15.95" customHeight="1"/>
+    <row r="248" ht="15.95" customHeight="1"/>
+    <row r="249" ht="15.95" customHeight="1"/>
+    <row r="250" ht="15.95" customHeight="1"/>
+    <row r="251" ht="15.95" customHeight="1"/>
+    <row r="252" ht="15.95" customHeight="1"/>
+    <row r="253" ht="15.95" customHeight="1"/>
+    <row r="254" ht="15.95" customHeight="1"/>
+    <row r="255" ht="15.95" customHeight="1"/>
+    <row r="256" ht="15.95" customHeight="1"/>
+    <row r="257" ht="15.95" customHeight="1"/>
+    <row r="258" ht="15.95" customHeight="1"/>
+    <row r="259" ht="15.95" customHeight="1"/>
+    <row r="260" ht="15.95" customHeight="1"/>
+    <row r="261" ht="15.95" customHeight="1"/>
+    <row r="262" ht="15.95" customHeight="1"/>
+    <row r="263" ht="15.95" customHeight="1"/>
+    <row r="264" ht="15.95" customHeight="1"/>
+    <row r="265" ht="15.95" customHeight="1"/>
+    <row r="266" ht="15.95" customHeight="1"/>
+    <row r="267" ht="15.95" customHeight="1"/>
+    <row r="268" ht="15.95" customHeight="1"/>
+    <row r="269" ht="15.95" customHeight="1"/>
+    <row r="270" ht="15.95" customHeight="1"/>
+    <row r="271" ht="15.95" customHeight="1"/>
+    <row r="272" ht="15.95" customHeight="1"/>
+    <row r="273" ht="15.95" customHeight="1"/>
+    <row r="274" ht="15.95" customHeight="1"/>
+    <row r="275" ht="15.95" customHeight="1"/>
+    <row r="276" ht="15.95" customHeight="1"/>
+    <row r="277" ht="15.95" customHeight="1"/>
+    <row r="278" ht="15.95" customHeight="1"/>
+    <row r="279" ht="15.95" customHeight="1"/>
+    <row r="280" ht="15.95" customHeight="1"/>
+    <row r="281" ht="15.95" customHeight="1"/>
+    <row r="282" ht="15.95" customHeight="1"/>
+    <row r="283" ht="15.95" customHeight="1"/>
+    <row r="284" ht="15.95" customHeight="1"/>
+    <row r="285" ht="15.95" customHeight="1"/>
+    <row r="286" ht="15.95" customHeight="1"/>
+    <row r="287" ht="15.95" customHeight="1"/>
+    <row r="288" ht="15.95" customHeight="1"/>
+    <row r="289" ht="15.95" customHeight="1"/>
+    <row r="290" ht="15.95" customHeight="1"/>
+    <row r="291" ht="15.95" customHeight="1"/>
+    <row r="292" ht="15.95" customHeight="1"/>
+    <row r="293" ht="15.95" customHeight="1"/>
+    <row r="294" ht="15.95" customHeight="1"/>
+    <row r="295" ht="15.95" customHeight="1"/>
+    <row r="296" ht="15.95" customHeight="1"/>
+    <row r="297" ht="15.95" customHeight="1"/>
+    <row r="298" ht="15.95" customHeight="1"/>
+    <row r="299" ht="15.95" customHeight="1"/>
+    <row r="300" ht="15.95" customHeight="1"/>
+    <row r="301" ht="15.95" customHeight="1"/>
+    <row r="302" ht="15.95" customHeight="1"/>
+    <row r="303" ht="15.95" customHeight="1"/>
+    <row r="304" ht="15.95" customHeight="1"/>
+    <row r="305" ht="15.95" customHeight="1"/>
+    <row r="306" ht="15.95" customHeight="1"/>
+    <row r="307" ht="15.95" customHeight="1"/>
+    <row r="308" ht="15.95" customHeight="1"/>
+    <row r="309" ht="15.95" customHeight="1"/>
+    <row r="310" ht="15.95" customHeight="1"/>
+    <row r="311" ht="15.95" customHeight="1"/>
+    <row r="312" ht="15.95" customHeight="1"/>
+    <row r="313" ht="15.95" customHeight="1"/>
+    <row r="314" ht="15.95" customHeight="1"/>
+    <row r="315" ht="15.95" customHeight="1"/>
+    <row r="316" ht="15.95" customHeight="1"/>
+    <row r="317" ht="15.95" customHeight="1"/>
+    <row r="318" ht="15.95" customHeight="1"/>
+    <row r="319" ht="15.95" customHeight="1"/>
+    <row r="320" ht="15.95" customHeight="1"/>
+    <row r="321" ht="15.95" customHeight="1"/>
+    <row r="322" ht="15.95" customHeight="1"/>
+    <row r="323" ht="15.95" customHeight="1"/>
+    <row r="324" ht="15.95" customHeight="1"/>
+    <row r="325" ht="15.95" customHeight="1"/>
+    <row r="326" ht="15.95" customHeight="1"/>
+    <row r="327" ht="15.95" customHeight="1"/>
+    <row r="328" ht="15.95" customHeight="1"/>
+    <row r="329" ht="15.95" customHeight="1"/>
+    <row r="330" ht="15.95" customHeight="1"/>
+    <row r="331" ht="15.95" customHeight="1"/>
+    <row r="332" ht="15.95" customHeight="1"/>
+    <row r="333" ht="15.95" customHeight="1"/>
+    <row r="334" ht="15.95" customHeight="1"/>
+    <row r="335" ht="15.95" customHeight="1"/>
+    <row r="336" ht="15.95" customHeight="1"/>
+    <row r="337" ht="15.95" customHeight="1"/>
+    <row r="338" ht="15.95" customHeight="1"/>
+    <row r="339" ht="15.95" customHeight="1"/>
+    <row r="340" ht="15.95" customHeight="1"/>
+    <row r="341" ht="15.95" customHeight="1"/>
+    <row r="342" ht="15.95" customHeight="1"/>
+    <row r="343" ht="15.95" customHeight="1"/>
+    <row r="344" ht="15.95" customHeight="1"/>
+    <row r="345" ht="15.95" customHeight="1"/>
+    <row r="346" ht="15.95" customHeight="1"/>
+    <row r="347" ht="15.95" customHeight="1"/>
+    <row r="348" ht="15.95" customHeight="1"/>
+    <row r="349" ht="15.95" customHeight="1"/>
+    <row r="350" ht="15.95" customHeight="1"/>
+    <row r="351" ht="15.95" customHeight="1"/>
+    <row r="352" ht="15.95" customHeight="1"/>
+    <row r="353" ht="15.95" customHeight="1"/>
+    <row r="354" ht="15.95" customHeight="1"/>
+    <row r="355" ht="15.95" customHeight="1"/>
+    <row r="356" ht="15.95" customHeight="1"/>
+    <row r="357" ht="15.95" customHeight="1"/>
+    <row r="358" ht="15.95" customHeight="1"/>
+    <row r="359" ht="15.95" customHeight="1"/>
+    <row r="360" ht="15.95" customHeight="1"/>
+    <row r="361" ht="15.95" customHeight="1"/>
+    <row r="362" ht="15.95" customHeight="1"/>
+    <row r="363" ht="15.95" customHeight="1"/>
+    <row r="364" ht="15.95" customHeight="1"/>
+    <row r="365" ht="15.95" customHeight="1"/>
+    <row r="366" ht="15.95" customHeight="1"/>
+    <row r="367" ht="15.95" customHeight="1"/>
+    <row r="368" ht="15.95" customHeight="1"/>
+    <row r="369" ht="15.95" customHeight="1"/>
+    <row r="370" ht="15.95" customHeight="1"/>
+    <row r="371" ht="15.95" customHeight="1"/>
+    <row r="372" ht="15.95" customHeight="1"/>
+    <row r="373" ht="15.95" customHeight="1"/>
+    <row r="374" ht="15.95" customHeight="1"/>
+    <row r="375" ht="15.95" customHeight="1"/>
+    <row r="376" ht="15.95" customHeight="1"/>
+    <row r="377" ht="15.95" customHeight="1"/>
+    <row r="378" ht="15.95" customHeight="1"/>
+    <row r="379" ht="15.95" customHeight="1"/>
+    <row r="380" ht="15.95" customHeight="1"/>
+    <row r="381" ht="15.95" customHeight="1"/>
+    <row r="382" ht="15.95" customHeight="1"/>
+    <row r="383" ht="15.95" customHeight="1"/>
+    <row r="384" ht="15.95" customHeight="1"/>
+    <row r="385" ht="15.95" customHeight="1"/>
+    <row r="386" ht="15.95" customHeight="1"/>
+    <row r="387" ht="15.95" customHeight="1"/>
+    <row r="388" ht="15.95" customHeight="1"/>
+    <row r="389" ht="15.95" customHeight="1"/>
+    <row r="390" ht="15.95" customHeight="1"/>
+    <row r="391" ht="15.95" customHeight="1"/>
+    <row r="392" ht="15.95" customHeight="1"/>
+    <row r="393" ht="15.95" customHeight="1"/>
+    <row r="394" ht="15.95" customHeight="1"/>
+    <row r="395" ht="15.95" customHeight="1"/>
+    <row r="396" ht="15.95" customHeight="1"/>
+    <row r="397" ht="15.95" customHeight="1"/>
+    <row r="398" ht="15.95" customHeight="1"/>
+    <row r="399" ht="15.95" customHeight="1"/>
+    <row r="400" ht="15.95" customHeight="1"/>
+    <row r="401" ht="15.95" customHeight="1"/>
+    <row r="402" ht="15.95" customHeight="1"/>
+    <row r="403" ht="15.95" customHeight="1"/>
+    <row r="404" ht="15.95" customHeight="1"/>
+    <row r="405" ht="15.95" customHeight="1"/>
+    <row r="406" ht="15.95" customHeight="1"/>
+    <row r="407" ht="15.95" customHeight="1"/>
+    <row r="408" ht="15.95" customHeight="1"/>
+    <row r="409" ht="15.95" customHeight="1"/>
+    <row r="410" ht="15.95" customHeight="1"/>
+    <row r="411" ht="15.95" customHeight="1"/>
+    <row r="412" ht="15.95" customHeight="1"/>
+    <row r="413" ht="15.95" customHeight="1"/>
+    <row r="414" ht="15.95" customHeight="1"/>
+    <row r="415" ht="15.95" customHeight="1"/>
+    <row r="416" ht="15.95" customHeight="1"/>
+    <row r="417" ht="15.95" customHeight="1"/>
+    <row r="418" ht="15.95" customHeight="1"/>
+    <row r="419" ht="15.95" customHeight="1"/>
+    <row r="420" ht="15.95" customHeight="1"/>
+    <row r="421" ht="15.95" customHeight="1"/>
+    <row r="422" ht="15.95" customHeight="1"/>
+    <row r="423" ht="15.95" customHeight="1"/>
+    <row r="424" ht="15.95" customHeight="1"/>
+    <row r="425" ht="15.95" customHeight="1"/>
+    <row r="426" ht="15.95" customHeight="1"/>
+    <row r="427" ht="15.95" customHeight="1"/>
+    <row r="428" ht="15.95" customHeight="1"/>
+    <row r="429" ht="15.95" customHeight="1"/>
+    <row r="430" ht="15.95" customHeight="1"/>
+    <row r="431" ht="15.95" customHeight="1"/>
+    <row r="432" ht="15.95" customHeight="1"/>
+    <row r="433" ht="15.95" customHeight="1"/>
+    <row r="434" ht="15.95" customHeight="1"/>
+    <row r="435" ht="15.95" customHeight="1"/>
+    <row r="436" ht="15.95" customHeight="1"/>
+    <row r="437" ht="15.95" customHeight="1"/>
+    <row r="438" ht="15.95" customHeight="1"/>
+    <row r="439" ht="15.95" customHeight="1"/>
+    <row r="440" ht="15.95" customHeight="1"/>
+    <row r="441" ht="15.95" customHeight="1"/>
+    <row r="442" ht="15.95" customHeight="1"/>
+    <row r="443" ht="15.95" customHeight="1"/>
+    <row r="444" ht="15.95" customHeight="1"/>
+    <row r="445" ht="15.95" customHeight="1"/>
+    <row r="446" ht="15.95" customHeight="1"/>
+    <row r="447" ht="15.95" customHeight="1"/>
+    <row r="448" ht="15.95" customHeight="1"/>
+    <row r="449" ht="15.95" customHeight="1"/>
+    <row r="450" ht="15.95" customHeight="1"/>
+    <row r="451" ht="15.95" customHeight="1"/>
+    <row r="452" ht="15.95" customHeight="1"/>
+    <row r="453" ht="15.95" customHeight="1"/>
+    <row r="454" ht="15.95" customHeight="1"/>
+    <row r="455" ht="15.95" customHeight="1"/>
+    <row r="456" ht="15.95" customHeight="1"/>
+    <row r="457" ht="15.95" customHeight="1"/>
+    <row r="458" ht="15.95" customHeight="1"/>
+    <row r="459" ht="15.95" customHeight="1"/>
+    <row r="460" ht="15.95" customHeight="1"/>
+    <row r="461" ht="15.95" customHeight="1"/>
+    <row r="462" ht="15.95" customHeight="1"/>
+    <row r="463" ht="15.95" customHeight="1"/>
+    <row r="464" ht="15.95" customHeight="1"/>
+    <row r="465" ht="15.95" customHeight="1"/>
+    <row r="466" ht="15.95" customHeight="1"/>
+    <row r="467" ht="15.95" customHeight="1"/>
+    <row r="468" ht="15.95" customHeight="1"/>
+    <row r="469" ht="15.95" customHeight="1"/>
+    <row r="470" ht="15.95" customHeight="1"/>
+    <row r="471" ht="15.95" customHeight="1"/>
+    <row r="472" ht="15.95" customHeight="1"/>
+    <row r="473" ht="15.95" customHeight="1"/>
+    <row r="474" ht="15.95" customHeight="1"/>
+    <row r="475" ht="15.95" customHeight="1"/>
+    <row r="476" ht="15.95" customHeight="1"/>
+    <row r="477" ht="15.95" customHeight="1"/>
+    <row r="478" ht="15.95" customHeight="1"/>
+    <row r="479" ht="15.95" customHeight="1"/>
+    <row r="480" ht="15.95" customHeight="1"/>
+    <row r="481" ht="15.95" customHeight="1"/>
+    <row r="482" ht="15.95" customHeight="1"/>
+    <row r="483" ht="15.95" customHeight="1"/>
+    <row r="484" ht="15.95" customHeight="1"/>
+    <row r="485" ht="15.95" customHeight="1"/>
+    <row r="486" ht="15.95" customHeight="1"/>
+    <row r="487" ht="15.95" customHeight="1"/>
+    <row r="488" ht="15.95" customHeight="1"/>
+    <row r="489" ht="15.95" customHeight="1"/>
+    <row r="490" ht="15.95" customHeight="1"/>
+    <row r="491" ht="15.95" customHeight="1"/>
+    <row r="492" ht="15.95" customHeight="1"/>
+    <row r="493" ht="15.95" customHeight="1"/>
+    <row r="494" ht="15.95" customHeight="1"/>
+    <row r="495" ht="15.95" customHeight="1"/>
+    <row r="496" ht="15.95" customHeight="1"/>
+    <row r="497" ht="15.95" customHeight="1"/>
+    <row r="498" ht="15.95" customHeight="1"/>
+    <row r="499" ht="15.95" customHeight="1"/>
+    <row r="500" ht="15.95" customHeight="1"/>
+    <row r="501" ht="15.95" customHeight="1"/>
+    <row r="502" ht="15.95" customHeight="1"/>
+    <row r="503" ht="15.95" customHeight="1"/>
+    <row r="504" ht="15.95" customHeight="1"/>
+    <row r="505" ht="15.95" customHeight="1"/>
+    <row r="506" ht="15.95" customHeight="1"/>
+    <row r="507" ht="15.95" customHeight="1"/>
+    <row r="508" ht="15.95" customHeight="1"/>
+    <row r="509" ht="15.95" customHeight="1"/>
+    <row r="510" ht="15.95" customHeight="1"/>
+    <row r="511" ht="15.95" customHeight="1"/>
+    <row r="512" ht="15.95" customHeight="1"/>
+    <row r="513" ht="15.95" customHeight="1"/>
+    <row r="514" ht="15.95" customHeight="1"/>
+    <row r="515" ht="15.95" customHeight="1"/>
+    <row r="516" ht="15.95" customHeight="1"/>
+    <row r="517" ht="15.95" customHeight="1"/>
+    <row r="518" ht="15.95" customHeight="1"/>
+    <row r="519" ht="15.95" customHeight="1"/>
+    <row r="520" ht="15.95" customHeight="1"/>
+    <row r="521" ht="15.95" customHeight="1"/>
+    <row r="522" ht="15.95" customHeight="1"/>
+    <row r="523" ht="15.95" customHeight="1"/>
+    <row r="524" ht="15.95" customHeight="1"/>
+    <row r="525" ht="15.95" customHeight="1"/>
+    <row r="526" ht="15.95" customHeight="1"/>
+    <row r="527" ht="15.95" customHeight="1"/>
+    <row r="528" ht="15.95" customHeight="1"/>
+    <row r="529" ht="15.95" customHeight="1"/>
+    <row r="530" ht="15.95" customHeight="1"/>
+    <row r="531" ht="15.95" customHeight="1"/>
+    <row r="532" ht="15.95" customHeight="1"/>
+    <row r="533" ht="15.95" customHeight="1"/>
+    <row r="534" ht="15.95" customHeight="1"/>
+    <row r="535" ht="15.95" customHeight="1"/>
+    <row r="536" ht="15.95" customHeight="1"/>
+    <row r="537" ht="15.95" customHeight="1"/>
+    <row r="538" ht="15.95" customHeight="1"/>
+    <row r="539" ht="15.95" customHeight="1"/>
+    <row r="540" ht="15.95" customHeight="1"/>
+    <row r="541" ht="15.95" customHeight="1"/>
+    <row r="542" ht="15.95" customHeight="1"/>
+    <row r="543" ht="15.95" customHeight="1"/>
+    <row r="544" ht="15.95" customHeight="1"/>
+    <row r="545" ht="15.95" customHeight="1"/>
+    <row r="546" ht="15.95" customHeight="1"/>
+    <row r="547" ht="15.95" customHeight="1"/>
+    <row r="548" ht="15.95" customHeight="1"/>
+    <row r="549" ht="15.95" customHeight="1"/>
+    <row r="550" ht="15.95" customHeight="1"/>
+    <row r="551" ht="15.95" customHeight="1"/>
+    <row r="552" ht="15.95" customHeight="1"/>
+    <row r="553" ht="15.95" customHeight="1"/>
+    <row r="554" ht="15.95" customHeight="1"/>
+    <row r="555" ht="15.95" customHeight="1"/>
+    <row r="556" ht="15.95" customHeight="1"/>
+    <row r="557" ht="15.95" customHeight="1"/>
+    <row r="558" ht="15.95" customHeight="1"/>
+    <row r="559" ht="15.95" customHeight="1"/>
+    <row r="560" ht="15.95" customHeight="1"/>
+    <row r="561" ht="15.95" customHeight="1"/>
+    <row r="562" ht="15.95" customHeight="1"/>
+    <row r="563" ht="15.95" customHeight="1"/>
+    <row r="564" ht="15.95" customHeight="1"/>
+    <row r="565" ht="15.95" customHeight="1"/>
+    <row r="566" ht="15.95" customHeight="1"/>
+    <row r="567" ht="15.95" customHeight="1"/>
+    <row r="568" ht="15.95" customHeight="1"/>
+    <row r="569" ht="15.95" customHeight="1"/>
+    <row r="570" ht="15.95" customHeight="1"/>
+    <row r="571" ht="15.95" customHeight="1"/>
+    <row r="572" ht="15.95" customHeight="1"/>
+    <row r="573" ht="15.95" customHeight="1"/>
+    <row r="574" ht="15.95" customHeight="1"/>
+    <row r="575" ht="15.95" customHeight="1"/>
+    <row r="576" ht="15.95" customHeight="1"/>
+    <row r="577" ht="15.95" customHeight="1"/>
+    <row r="578" ht="15.95" customHeight="1"/>
+    <row r="579" ht="15.95" customHeight="1"/>
+    <row r="580" ht="15.95" customHeight="1"/>
+    <row r="581" ht="15.95" customHeight="1"/>
+    <row r="582" ht="15.95" customHeight="1"/>
+    <row r="583" ht="15.95" customHeight="1"/>
+    <row r="584" ht="15.95" customHeight="1"/>
+    <row r="585" ht="15.95" customHeight="1"/>
+    <row r="586" ht="15.95" customHeight="1"/>
+    <row r="587" ht="15.95" customHeight="1"/>
+    <row r="588" ht="15.95" customHeight="1"/>
+    <row r="589" ht="15.95" customHeight="1"/>
+    <row r="590" ht="15.95" customHeight="1"/>
+    <row r="591" ht="15.95" customHeight="1"/>
+    <row r="592" ht="15.95" customHeight="1"/>
+    <row r="593" ht="15.95" customHeight="1"/>
+    <row r="594" ht="15.95" customHeight="1"/>
+    <row r="595" ht="15.95" customHeight="1"/>
+    <row r="596" ht="15.95" customHeight="1"/>
+    <row r="597" ht="15.95" customHeight="1"/>
+    <row r="598" ht="15.95" customHeight="1"/>
+    <row r="599" ht="15.95" customHeight="1"/>
+    <row r="600" ht="15.95" customHeight="1"/>
+    <row r="601" ht="15.95" customHeight="1"/>
+    <row r="602" ht="15.95" customHeight="1"/>
+    <row r="603" ht="15.95" customHeight="1"/>
+    <row r="604" ht="15.95" customHeight="1"/>
+    <row r="605" ht="15.95" customHeight="1"/>
+    <row r="606" ht="15.95" customHeight="1"/>
+    <row r="607" ht="15.95" customHeight="1"/>
+    <row r="608" ht="15.95" customHeight="1"/>
+    <row r="609" ht="15.95" customHeight="1"/>
+    <row r="610" ht="15.95" customHeight="1"/>
+    <row r="611" ht="15.95" customHeight="1"/>
+    <row r="612" ht="15.95" customHeight="1"/>
+    <row r="613" ht="15.95" customHeight="1"/>
+    <row r="614" ht="15.95" customHeight="1"/>
+    <row r="615" ht="15.95" customHeight="1"/>
+    <row r="616" ht="15.95" customHeight="1"/>
+    <row r="617" ht="15.95" customHeight="1"/>
+    <row r="618" ht="15.95" customHeight="1"/>
+    <row r="619" ht="15.95" customHeight="1"/>
+    <row r="620" ht="15.95" customHeight="1"/>
+    <row r="621" ht="15.95" customHeight="1"/>
+    <row r="622" ht="15.95" customHeight="1"/>
+    <row r="623" ht="15.95" customHeight="1"/>
+    <row r="624" ht="15.95" customHeight="1"/>
+    <row r="625" ht="15.95" customHeight="1"/>
+    <row r="626" ht="15.95" customHeight="1"/>
+    <row r="627" ht="15.95" customHeight="1"/>
+    <row r="628" ht="15.95" customHeight="1"/>
+    <row r="629" ht="15.95" customHeight="1"/>
+    <row r="630" ht="15.95" customHeight="1"/>
+    <row r="631" ht="15.95" customHeight="1"/>
+    <row r="632" ht="15.95" customHeight="1"/>
+    <row r="633" ht="15.95" customHeight="1"/>
+    <row r="634" ht="15.95" customHeight="1"/>
+    <row r="635" ht="15.95" customHeight="1"/>
+    <row r="636" ht="15.95" customHeight="1"/>
+    <row r="637" ht="15.95" customHeight="1"/>
+    <row r="638" ht="15.95" customHeight="1"/>
+    <row r="639" ht="15.95" customHeight="1"/>
+    <row r="640" ht="15.95" customHeight="1"/>
+    <row r="641" ht="15.95" customHeight="1"/>
+    <row r="642" ht="15.95" customHeight="1"/>
+    <row r="643" ht="15.95" customHeight="1"/>
+    <row r="644" ht="15.95" customHeight="1"/>
+    <row r="645" ht="15.95" customHeight="1"/>
+    <row r="646" ht="15.95" customHeight="1"/>
+    <row r="647" ht="15.95" customHeight="1"/>
+    <row r="648" ht="15.95" customHeight="1"/>
+    <row r="649" ht="15.95" customHeight="1"/>
+    <row r="650" ht="15.95" customHeight="1"/>
+    <row r="651" ht="15.95" customHeight="1"/>
+    <row r="652" ht="15.95" customHeight="1"/>
+    <row r="653" ht="15.95" customHeight="1"/>
+    <row r="654" ht="15.95" customHeight="1"/>
+    <row r="655" ht="15.95" customHeight="1"/>
+    <row r="656" ht="15.95" customHeight="1"/>
+    <row r="657" ht="15.95" customHeight="1"/>
+    <row r="658" ht="15.95" customHeight="1"/>
+    <row r="659" ht="15.95" customHeight="1"/>
+    <row r="660" ht="15.95" customHeight="1"/>
+    <row r="661" ht="15.95" customHeight="1"/>
+    <row r="662" ht="15.95" customHeight="1"/>
+    <row r="663" ht="15.95" customHeight="1"/>
+    <row r="664" ht="15.95" customHeight="1"/>
+    <row r="665" ht="15.95" customHeight="1"/>
+    <row r="666" ht="15.95" customHeight="1"/>
+    <row r="667" ht="15.95" customHeight="1"/>
+    <row r="668" ht="15.95" customHeight="1"/>
+    <row r="669" ht="15.95" customHeight="1"/>
+    <row r="670" ht="15.95" customHeight="1"/>
+    <row r="671" ht="15.95" customHeight="1"/>
+    <row r="672" ht="15.95" customHeight="1"/>
+    <row r="673" ht="15.95" customHeight="1"/>
+    <row r="674" ht="15.95" customHeight="1"/>
+    <row r="675" ht="15.95" customHeight="1"/>
+    <row r="676" ht="15.95" customHeight="1"/>
+    <row r="677" ht="15.95" customHeight="1"/>
+    <row r="678" ht="15.95" customHeight="1"/>
+    <row r="679" ht="15.95" customHeight="1"/>
+    <row r="680" ht="15.95" customHeight="1"/>
+    <row r="681" ht="15.95" customHeight="1"/>
+    <row r="682" ht="15.95" customHeight="1"/>
+    <row r="683" ht="15.95" customHeight="1"/>
+    <row r="684" ht="15.95" customHeight="1"/>
+    <row r="685" ht="15.95" customHeight="1"/>
+    <row r="686" ht="15.95" customHeight="1"/>
+    <row r="687" ht="15.95" customHeight="1"/>
+    <row r="688" ht="15.95" customHeight="1"/>
+    <row r="689" ht="15.95" customHeight="1"/>
+    <row r="690" ht="15.95" customHeight="1"/>
+    <row r="691" ht="15.95" customHeight="1"/>
+    <row r="692" ht="15.95" customHeight="1"/>
+    <row r="693" ht="15.95" customHeight="1"/>
+    <row r="694" ht="15.95" customHeight="1"/>
+    <row r="695" ht="15.95" customHeight="1"/>
+    <row r="696" ht="15.95" customHeight="1"/>
+    <row r="697" ht="15.95" customHeight="1"/>
+    <row r="698" ht="15.95" customHeight="1"/>
+    <row r="699" ht="15.95" customHeight="1"/>
+    <row r="700" ht="15.95" customHeight="1"/>
+    <row r="701" ht="15.95" customHeight="1"/>
+    <row r="702" ht="15.95" customHeight="1"/>
+    <row r="703" ht="15.95" customHeight="1"/>
+    <row r="704" ht="15.95" customHeight="1"/>
+    <row r="705" ht="15.95" customHeight="1"/>
+    <row r="706" ht="15.95" customHeight="1"/>
+    <row r="707" ht="15.95" customHeight="1"/>
+    <row r="708" ht="15.95" customHeight="1"/>
+    <row r="709" ht="15.95" customHeight="1"/>
+    <row r="710" ht="15.95" customHeight="1"/>
+    <row r="711" ht="15.95" customHeight="1"/>
+    <row r="712" ht="15.95" customHeight="1"/>
+    <row r="713" ht="15.95" customHeight="1"/>
+    <row r="714" ht="15.95" customHeight="1"/>
+    <row r="715" ht="15.95" customHeight="1"/>
+    <row r="716" ht="15.95" customHeight="1"/>
+    <row r="717" ht="15.95" customHeight="1"/>
+    <row r="718" ht="15.95" customHeight="1"/>
+    <row r="719" ht="15.95" customHeight="1"/>
+    <row r="720" ht="15.95" customHeight="1"/>
+    <row r="721" ht="15.95" customHeight="1"/>
+    <row r="722" ht="15.95" customHeight="1"/>
+    <row r="723" ht="15.95" customHeight="1"/>
+    <row r="724" ht="15.95" customHeight="1"/>
+    <row r="725" ht="15.95" customHeight="1"/>
+    <row r="726" ht="15.95" customHeight="1"/>
+    <row r="727" ht="15.95" customHeight="1"/>
+    <row r="728" ht="15.95" customHeight="1"/>
+    <row r="729" ht="15.95" customHeight="1"/>
+    <row r="730" ht="15.95" customHeight="1"/>
+    <row r="731" ht="15.95" customHeight="1"/>
+    <row r="732" ht="15.95" customHeight="1"/>
+    <row r="733" ht="15.95" customHeight="1"/>
+    <row r="734" ht="15.95" customHeight="1"/>
+    <row r="735" ht="15.95" customHeight="1"/>
+    <row r="736" ht="15.95" customHeight="1"/>
+    <row r="737" ht="15.95" customHeight="1"/>
+    <row r="738" ht="15.95" customHeight="1"/>
+    <row r="739" ht="15.95" customHeight="1"/>
+    <row r="740" ht="15.95" customHeight="1"/>
+    <row r="741" ht="15.95" customHeight="1"/>
+    <row r="742" ht="15.95" customHeight="1"/>
+    <row r="743" ht="15.95" customHeight="1"/>
+    <row r="744" ht="15.95" customHeight="1"/>
+    <row r="745" ht="15.95" customHeight="1"/>
+    <row r="746" ht="15.95" customHeight="1"/>
+    <row r="747" ht="15.95" customHeight="1"/>
+    <row r="748" ht="15.95" customHeight="1"/>
+    <row r="749" ht="15.95" customHeight="1"/>
+    <row r="750" ht="15.95" customHeight="1"/>
+    <row r="751" ht="15.95" customHeight="1"/>
+    <row r="752" ht="15.95" customHeight="1"/>
+    <row r="753" ht="15.95" customHeight="1"/>
+    <row r="754" ht="15.95" customHeight="1"/>
+    <row r="755" ht="15.95" customHeight="1"/>
+    <row r="756" ht="15.95" customHeight="1"/>
+    <row r="757" ht="15.95" customHeight="1"/>
+    <row r="758" ht="15.95" customHeight="1"/>
+    <row r="759" ht="15.95" customHeight="1"/>
+    <row r="760" ht="15.95" customHeight="1"/>
+    <row r="761" ht="15.95" customHeight="1"/>
+    <row r="762" ht="15.95" customHeight="1"/>
+    <row r="763" ht="15.95" customHeight="1"/>
+    <row r="764" ht="15.95" customHeight="1"/>
+    <row r="765" ht="15.95" customHeight="1"/>
+    <row r="766" ht="15.95" customHeight="1"/>
+    <row r="767" ht="15.95" customHeight="1"/>
+    <row r="768" ht="15.95" customHeight="1"/>
+    <row r="769" ht="15.95" customHeight="1"/>
+    <row r="770" ht="15.95" customHeight="1"/>
+    <row r="771" ht="15.95" customHeight="1"/>
+    <row r="772" ht="15.95" customHeight="1"/>
+    <row r="773" ht="15.95" customHeight="1"/>
+    <row r="774" ht="15.95" customHeight="1"/>
+    <row r="775" ht="15.95" customHeight="1"/>
+    <row r="776" ht="15.95" customHeight="1"/>
+    <row r="777" ht="15.95" customHeight="1"/>
+    <row r="778" ht="15.95" customHeight="1"/>
+    <row r="779" ht="15.95" customHeight="1"/>
+    <row r="780" ht="15.95" customHeight="1"/>
+    <row r="781" ht="15.95" customHeight="1"/>
+    <row r="782" ht="15.95" customHeight="1"/>
+    <row r="783" ht="15.95" customHeight="1"/>
+    <row r="784" ht="15.95" customHeight="1"/>
+    <row r="785" ht="15.95" customHeight="1"/>
+    <row r="786" ht="15.95" customHeight="1"/>
+    <row r="787" ht="15.95" customHeight="1"/>
+    <row r="788" ht="15.95" customHeight="1"/>
+    <row r="789" ht="15.95" customHeight="1"/>
+    <row r="790" ht="15.95" customHeight="1"/>
+    <row r="791" ht="15.95" customHeight="1"/>
+    <row r="792" ht="15.95" customHeight="1"/>
+    <row r="793" ht="15.95" customHeight="1"/>
+    <row r="794" ht="15.95" customHeight="1"/>
+    <row r="795" ht="15.95" customHeight="1"/>
+    <row r="796" ht="15.95" customHeight="1"/>
+    <row r="797" ht="15.95" customHeight="1"/>
+    <row r="798" ht="15.95" customHeight="1"/>
+    <row r="799" ht="15.95" customHeight="1"/>
+    <row r="800" ht="15.95" customHeight="1"/>
+    <row r="801" ht="15.95" customHeight="1"/>
+    <row r="802" ht="15.95" customHeight="1"/>
+    <row r="803" ht="15.95" customHeight="1"/>
+    <row r="804" ht="15.95" customHeight="1"/>
+    <row r="805" ht="15.95" customHeight="1"/>
+    <row r="806" ht="15.95" customHeight="1"/>
+    <row r="807" ht="15.95" customHeight="1"/>
+    <row r="808" ht="15.95" customHeight="1"/>
+    <row r="809" ht="15.95" customHeight="1"/>
+    <row r="810" ht="15.95" customHeight="1"/>
+    <row r="811" ht="15.95" customHeight="1"/>
+    <row r="812" ht="15.95" customHeight="1"/>
+    <row r="813" ht="15.95" customHeight="1"/>
+    <row r="814" ht="15.95" customHeight="1"/>
+    <row r="815" ht="15.95" customHeight="1"/>
+    <row r="816" ht="15.95" customHeight="1"/>
+    <row r="817" ht="15.95" customHeight="1"/>
+    <row r="818" ht="15.95" customHeight="1"/>
+    <row r="819" ht="15.95" customHeight="1"/>
+    <row r="820" ht="15.95" customHeight="1"/>
+    <row r="821" ht="15.95" customHeight="1"/>
+    <row r="822" ht="15.95" customHeight="1"/>
+    <row r="823" ht="15.95" customHeight="1"/>
+    <row r="824" ht="15.95" customHeight="1"/>
+    <row r="825" ht="15.95" customHeight="1"/>
+    <row r="826" ht="15.95" customHeight="1"/>
+    <row r="827" ht="15.95" customHeight="1"/>
+    <row r="828" ht="15.95" customHeight="1"/>
+    <row r="829" ht="15.95" customHeight="1"/>
+    <row r="830" ht="15.95" customHeight="1"/>
+    <row r="831" ht="15.95" customHeight="1"/>
+    <row r="832" ht="15.95" customHeight="1"/>
+    <row r="833" ht="15.95" customHeight="1"/>
+    <row r="834" ht="15.95" customHeight="1"/>
+    <row r="835" ht="15.95" customHeight="1"/>
+    <row r="836" ht="15.95" customHeight="1"/>
+    <row r="837" ht="15.95" customHeight="1"/>
+    <row r="838" ht="15.95" customHeight="1"/>
+    <row r="839" ht="15.95" customHeight="1"/>
+    <row r="840" ht="15.95" customHeight="1"/>
+    <row r="841" ht="15.95" customHeight="1"/>
+    <row r="842" ht="15.95" customHeight="1"/>
+    <row r="843" ht="15.95" customHeight="1"/>
+    <row r="844" ht="15.95" customHeight="1"/>
+    <row r="845" ht="15.95" customHeight="1"/>
+    <row r="846" ht="15.95" customHeight="1"/>
+    <row r="847" ht="15.95" customHeight="1"/>
+    <row r="848" ht="15.95" customHeight="1"/>
+    <row r="849" ht="15.95" customHeight="1"/>
+    <row r="850" ht="15.95" customHeight="1"/>
+    <row r="851" ht="15.95" customHeight="1"/>
+    <row r="852" ht="15.95" customHeight="1"/>
+    <row r="853" ht="15.95" customHeight="1"/>
+    <row r="854" ht="15.95" customHeight="1"/>
+    <row r="855" ht="15.95" customHeight="1"/>
+    <row r="856" ht="15.95" customHeight="1"/>
+    <row r="857" ht="15.95" customHeight="1"/>
+    <row r="858" ht="15.95" customHeight="1"/>
+    <row r="859" ht="15.95" customHeight="1"/>
+    <row r="860" ht="15.95" customHeight="1"/>
+    <row r="861" ht="15.95" customHeight="1"/>
+    <row r="862" ht="15.95" customHeight="1"/>
+    <row r="863" ht="15.95" customHeight="1"/>
+    <row r="864" ht="15.95" customHeight="1"/>
+    <row r="865" ht="15.95" customHeight="1"/>
+    <row r="866" ht="15.95" customHeight="1"/>
+    <row r="867" ht="15.95" customHeight="1"/>
+    <row r="868" ht="15.95" customHeight="1"/>
+    <row r="869" ht="15.95" customHeight="1"/>
+    <row r="870" ht="15.95" customHeight="1"/>
+    <row r="871" ht="15.95" customHeight="1"/>
+    <row r="872" ht="15.95" customHeight="1"/>
+    <row r="873" ht="15.95" customHeight="1"/>
+    <row r="874" ht="15.95" customHeight="1"/>
+    <row r="875" ht="15.95" customHeight="1"/>
+    <row r="876" ht="15.95" customHeight="1"/>
+    <row r="877" ht="15.95" customHeight="1"/>
+    <row r="878" ht="15.95" customHeight="1"/>
+    <row r="879" ht="15.95" customHeight="1"/>
+    <row r="880" ht="15.95" customHeight="1"/>
+    <row r="881" ht="15.95" customHeight="1"/>
+    <row r="882" ht="15.95" customHeight="1"/>
+    <row r="883" ht="15.95" customHeight="1"/>
+    <row r="884" ht="15.95" customHeight="1"/>
+    <row r="885" ht="15.95" customHeight="1"/>
+    <row r="886" ht="15.95" customHeight="1"/>
+    <row r="887" ht="15.95" customHeight="1"/>
+    <row r="888" ht="15.95" customHeight="1"/>
+    <row r="889" ht="15.95" customHeight="1"/>
+    <row r="890" ht="15.95" customHeight="1"/>
+    <row r="891" ht="15.95" customHeight="1"/>
+    <row r="892" ht="15.95" customHeight="1"/>
+    <row r="893" ht="15.95" customHeight="1"/>
+    <row r="894" ht="15.95" customHeight="1"/>
+    <row r="895" ht="15.95" customHeight="1"/>
+    <row r="896" ht="15.95" customHeight="1"/>
+    <row r="897" ht="15.95" customHeight="1"/>
+    <row r="898" ht="15.95" customHeight="1"/>
+    <row r="899" ht="15.95" customHeight="1"/>
+    <row r="900" ht="15.95" customHeight="1"/>
+    <row r="901" ht="15.95" customHeight="1"/>
+    <row r="902" ht="15.95" customHeight="1"/>
+    <row r="903" ht="15.95" customHeight="1"/>
+    <row r="904" ht="15.95" customHeight="1"/>
+    <row r="905" ht="15.95" customHeight="1"/>
+    <row r="906" ht="15.95" customHeight="1"/>
+    <row r="907" ht="15.95" customHeight="1"/>
+    <row r="908" ht="15.95" customHeight="1"/>
+    <row r="909" ht="15.95" customHeight="1"/>
+    <row r="910" ht="15.95" customHeight="1"/>
+    <row r="911" ht="15.95" customHeight="1"/>
+    <row r="912" ht="15.95" customHeight="1"/>
+    <row r="913" ht="15.95" customHeight="1"/>
+    <row r="914" ht="15.95" customHeight="1"/>
+    <row r="915" ht="15.95" customHeight="1"/>
+    <row r="916" ht="15.95" customHeight="1"/>
+    <row r="917" ht="15.95" customHeight="1"/>
+    <row r="918" ht="15.95" customHeight="1"/>
+    <row r="919" ht="15.95" customHeight="1"/>
+    <row r="920" ht="15.95" customHeight="1"/>
+    <row r="921" ht="15.95" customHeight="1"/>
+    <row r="922" ht="15.95" customHeight="1"/>
+    <row r="923" ht="15.95" customHeight="1"/>
+    <row r="924" ht="15.95" customHeight="1"/>
+    <row r="925" ht="15.95" customHeight="1"/>
+    <row r="926" ht="15.95" customHeight="1"/>
+    <row r="927" ht="15.95" customHeight="1"/>
+    <row r="928" ht="15.95" customHeight="1"/>
+    <row r="929" ht="15.95" customHeight="1"/>
+    <row r="930" ht="15.95" customHeight="1"/>
+    <row r="931" ht="15.95" customHeight="1"/>
+    <row r="932" ht="15.95" customHeight="1"/>
+    <row r="933" ht="15.95" customHeight="1"/>
+    <row r="934" ht="15.95" customHeight="1"/>
+    <row r="935" ht="15.95" customHeight="1"/>
+    <row r="936" ht="15.95" customHeight="1"/>
+    <row r="937" ht="15.95" customHeight="1"/>
+    <row r="938" ht="15.95" customHeight="1"/>
+    <row r="939" ht="15.95" customHeight="1"/>
+    <row r="940" ht="15.95" customHeight="1"/>
+    <row r="941" ht="15.95" customHeight="1"/>
+    <row r="942" ht="15.95" customHeight="1"/>
+    <row r="943" ht="15.95" customHeight="1"/>
+    <row r="944" ht="15.95" customHeight="1"/>
+    <row r="945" ht="15.95" customHeight="1"/>
+    <row r="946" ht="15.95" customHeight="1"/>
+    <row r="947" ht="15.95" customHeight="1"/>
+    <row r="948" ht="15.95" customHeight="1"/>
+    <row r="949" ht="15.95" customHeight="1"/>
+    <row r="950" ht="15.95" customHeight="1"/>
+    <row r="951" ht="15.95" customHeight="1"/>
+    <row r="952" ht="15.95" customHeight="1"/>
+    <row r="953" ht="15.95" customHeight="1"/>
+    <row r="954" ht="15.95" customHeight="1"/>
+    <row r="955" ht="15.95" customHeight="1"/>
+    <row r="956" ht="15.95" customHeight="1"/>
+    <row r="957" ht="15.95" customHeight="1"/>
+    <row r="958" ht="15.95" customHeight="1"/>
+    <row r="959" ht="15.95" customHeight="1"/>
+    <row r="960" ht="15.95" customHeight="1"/>
+    <row r="961" ht="15.95" customHeight="1"/>
+    <row r="962" ht="15.95" customHeight="1"/>
+    <row r="963" ht="15.95" customHeight="1"/>
+    <row r="964" ht="15.95" customHeight="1"/>
+    <row r="965" ht="15.95" customHeight="1"/>
+    <row r="966" ht="15.95" customHeight="1"/>
+    <row r="967" ht="15.95" customHeight="1"/>
+    <row r="968" ht="15.95" customHeight="1"/>
+    <row r="969" ht="15.95" customHeight="1"/>
+    <row r="970" ht="15.95" customHeight="1"/>
+    <row r="971" ht="15.95" customHeight="1"/>
+    <row r="972" ht="15.95" customHeight="1"/>
+    <row r="973" ht="15.95" customHeight="1"/>
+    <row r="974" ht="15.95" customHeight="1"/>
+    <row r="975" ht="15.95" customHeight="1"/>
+    <row r="976" ht="15.95" customHeight="1"/>
+    <row r="977" ht="15.95" customHeight="1"/>
+    <row r="978" ht="15.95" customHeight="1"/>
+    <row r="979" ht="15.95" customHeight="1"/>
+    <row r="980" ht="15.95" customHeight="1"/>
+    <row r="981" ht="15.95" customHeight="1"/>
+    <row r="982" ht="15.95" customHeight="1"/>
+    <row r="983" ht="15.95" customHeight="1"/>
+    <row r="984" ht="15.95" customHeight="1"/>
+    <row r="985" ht="15.95" customHeight="1"/>
+    <row r="986" ht="15.95" customHeight="1"/>
+    <row r="987" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:A4"/>
@@ -6879,30 +6749,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BFAF30-6EFD-4A13-A39A-D09455CAAF60}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12">
       <c r="A1" s="32" t="s">
         <v>83</v>
       </c>
@@ -6918,7 +6788,7 @@
       <c r="K1" s="33"/>
       <c r="L1" s="33"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12">
       <c r="A2" s="22" t="s">
         <v>84</v>
       </c>
@@ -6956,7 +6826,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15.6" customHeight="1">
       <c r="A3" s="23" t="s">
         <v>94</v>
       </c>
@@ -6993,12 +6863,39 @@
       <c r="L3" s="28" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="22"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POCOR-7382: code enahnce remove column , no need | Status: Done
</commit_message>
<xml_diff>
--- a/webroot/export/customexcel/default_templates/class_profile_template.xlsx
+++ b/webroot/export/customexcel/default_templates/class_profile_template.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Student Performance Summary" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>${"image":{"displayValue":"Institutions.logo_content","imageWidth":"100","imageMarginLeft":"20","imageMarginTop":"5"}}</t>
   </si>
@@ -334,25 +333,13 @@
   </si>
   <si>
     <t>${"match": {"displayValue": "StudentDetails.absence_day","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>Institution Average Mark</t>
-  </si>
-  <si>
-    <t>Area Average Mark</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.institution_average_mark","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
-  </si>
-  <si>
-    <t>${"match": {"displayValue": "StudentDetails.area_average_mark","rows": {"matchFrom": "StudentDetails.id","matchTo": "StudentDetails.id"}}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -410,21 +397,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF172B4D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,12 +540,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -586,10 +552,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -986,7 +952,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
@@ -1007,13 +973,13 @@
       <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
       <c r="H2" s="6"/>
@@ -1267,13 +1233,13 @@
       <c r="IV2" s="2"/>
     </row>
     <row r="3" spans="1:256" ht="25.5" customHeight="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="6"/>
@@ -1527,7 +1493,7 @@
       <c r="IV3" s="2"/>
     </row>
     <row r="4" spans="1:256" ht="22.5" customHeight="1">
-      <c r="A4" s="29"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -6750,10 +6716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -6767,28 +6733,24 @@
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:10">
       <c r="A2" s="22" t="s">
         <v>84</v>
       </c>
@@ -6816,17 +6778,11 @@
       <c r="I2" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" customHeight="1">
+    <row r="3" spans="1:10" ht="15.6" customHeight="1">
       <c r="A3" s="23" t="s">
         <v>94</v>
       </c>
@@ -6854,17 +6810,11 @@
       <c r="I3" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="L3" s="28" t="s">
+      <c r="J3" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:10">
       <c r="A50" s="22"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -6874,11 +6824,9 @@
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="22"/>
+      <c r="J50" s="22"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:10">
       <c r="A51" s="23"/>
       <c r="B51" s="24"/>
       <c r="C51" s="25"/>
@@ -6888,13 +6836,11 @@
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
       <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
+      <c r="J51" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>